<commit_message>
remove note in mothly report template
</commit_message>
<xml_diff>
--- a/job/templates/MonthlyReport-v1.xlsx
+++ b/job/templates/MonthlyReport-v1.xlsx
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Project</t>
   </si>
@@ -280,9 +280,6 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>1) Measured Energy (kWh) were taken from the SCADA.  The Measured Energy (kWh) and Weather Performance  are only preliminary and not audited.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Weather </t>
   </si>
   <si>
@@ -301,8 +298,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="[$-409]mmm\-yy;@"/>
-    <numFmt numFmtId="169" formatCode="[$-1010409]###,###"/>
+    <numFmt numFmtId="165" formatCode="[$-409]mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-1010409]###,###"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -933,8 +930,8 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="85">
@@ -952,7 +949,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -964,7 +961,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -985,7 +982,7 @@
     <xf numFmtId="9" fontId="9" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1018,25 +1015,25 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="9" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1093,7 +1090,7 @@
     <xf numFmtId="3" fontId="9" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="15" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1108,11 +1105,29 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1123,6 +1138,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1132,48 +1156,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1182,6 +1164,21 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1464,7 +1461,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1478,7 +1475,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B1" sqref="B1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1494,35 +1491,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="77.25" customHeight="1" thickBot="1">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="62"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="68"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="16.2" thickBot="1">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="70"/>
-      <c r="F2" s="71" t="s">
+      <c r="E2" s="79"/>
+      <c r="F2" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="82"/>
       <c r="I2" s="83" t="s">
         <v>4</v>
       </c>
@@ -1530,8 +1527,8 @@
       <c r="K2" s="84"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1">
-      <c r="B3" s="64"/>
-      <c r="C3" s="67"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="70"/>
       <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1554,12 +1551,12 @@
         <v>3</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1">
-      <c r="B4" s="65"/>
-      <c r="C4" s="68"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="71"/>
       <c r="D4" s="7" t="s">
         <v>9</v>
       </c>
@@ -1582,7 +1579,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="22.8">
@@ -1590,7 +1587,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="31">
         <v>42767</v>
@@ -1629,7 +1626,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="17">
         <v>42767</v>
@@ -1837,44 +1834,42 @@
       </c>
     </row>
     <row r="17" spans="2:11">
-      <c r="B17" s="80" t="s">
+      <c r="B17" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
-      <c r="E17" s="81"/>
-      <c r="F17" s="81"/>
-      <c r="G17" s="81"/>
-      <c r="H17" s="81"/>
-      <c r="I17" s="81"/>
-      <c r="J17" s="81"/>
-      <c r="K17" s="82"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="76"/>
+      <c r="J17" s="76"/>
+      <c r="K17" s="77"/>
     </row>
     <row r="18" spans="2:11">
-      <c r="B18" s="77" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="78"/>
-      <c r="J18" s="78"/>
-      <c r="K18" s="79"/>
+      <c r="B18" s="63"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="65"/>
     </row>
     <row r="19" spans="2:11" ht="15" thickBot="1">
-      <c r="B19" s="74"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="76"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="62"/>
     </row>
     <row r="20" spans="2:11">
       <c r="B20" s="18"/>

</xml_diff>

<commit_message>
remove comment in monthly report template
</commit_message>
<xml_diff>
--- a/job/templates/MonthlyReport-v1.xlsx
+++ b/job/templates/MonthlyReport-v1.xlsx
@@ -19,103 +19,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>astejada</author>
-  </authors>
-  <commentList>
-    <comment ref="G5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>astejada:
-("MEASURED INSOLATION"/INSOLATION REFERENCE") * (REFERENCE PRODUCTION KWH)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>astejada:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-"MEASURED PRODUCTION" / "REFERENCE PRODUCTION"</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>astejada:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-"MEASURED PRODUCTION" / "EXPECTED PRODUCTION"</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>astejada:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-"EXPECTED KWH" / "REFERENCE KWH"</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -301,7 +204,7 @@
     <numFmt numFmtId="165" formatCode="[$-409]mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="[$-1010409]###,###"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,19 +318,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1461,7 +1351,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1895,10 +1785,9 @@
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:K2"/>
   </mergeCells>
-  <phoneticPr fontId="19" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="83" orientation="landscape" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
monthly report excel template change
</commit_message>
<xml_diff>
--- a/job/templates/MonthlyReport-v1.xlsx
+++ b/job/templates/MonthlyReport-v1.xlsx
@@ -10,7 +10,7 @@
     <sheet name="February FireLight Ground Mount" sheetId="18" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'February FireLight Ground Mount'!$B$1:$K$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'February FireLight Ground Mount'!$B$1:$K$31</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -1351,7 +1351,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1362,10 +1362,10 @@
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K1"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1730,117 +1730,237 @@
       <c r="J18" s="20"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:11" ht="23.4" thickBot="1">
+    <row r="19" spans="1:11" ht="22.8">
       <c r="A19">
         <v>15</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="27"/>
-    </row>
-    <row r="20" spans="1:11" ht="23.4" thickBot="1">
-      <c r="B20" s="58" t="s">
+      <c r="B19" s="29"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="21"/>
+    </row>
+    <row r="20" spans="1:11" ht="22.8">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="21"/>
+    </row>
+    <row r="21" spans="1:11" ht="22.8">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="21"/>
+    </row>
+    <row r="22" spans="1:11" ht="22.8">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="21"/>
+    </row>
+    <row r="23" spans="1:11" ht="22.8">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="21"/>
+    </row>
+    <row r="24" spans="1:11" ht="22.8">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="21"/>
+    </row>
+    <row r="25" spans="1:11" ht="22.8">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25" s="29"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="21"/>
+    </row>
+    <row r="26" spans="1:11" ht="22.8">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="21"/>
+    </row>
+    <row r="27" spans="1:11" ht="23.4" thickBot="1">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" s="30"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="27"/>
+    </row>
+    <row r="28" spans="1:11" ht="23.4" thickBot="1">
+      <c r="B28" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="54">
-        <f>SUM(D5:D19)</f>
+      <c r="C28" s="53"/>
+      <c r="D28" s="54">
+        <f>SUM(D5:D27)</f>
         <v>200.12</v>
       </c>
-      <c r="E20" s="55">
-        <f>SUM(E5:E19)</f>
+      <c r="E28" s="55">
+        <f>SUM(E5:E27)</f>
         <v>175</v>
       </c>
-      <c r="F20" s="54">
-        <f>SUM(F5:F19)</f>
+      <c r="F28" s="54">
+        <f>SUM(F5:F27)</f>
         <v>158000</v>
       </c>
-      <c r="G20" s="22">
-        <f>SUM(G5:G19)</f>
+      <c r="G28" s="22">
+        <f>SUM(G5:G27)</f>
         <v>203424.34673856208</v>
       </c>
-      <c r="H20" s="55">
-        <f>SUM(H5:H19)</f>
+      <c r="H28" s="55">
+        <f>SUM(H5:H27)</f>
         <v>178026</v>
       </c>
-      <c r="I20" s="23">
-        <f>F20/H20</f>
+      <c r="I28" s="23">
+        <f>F28/H28</f>
         <v>0.88751081302731061</v>
       </c>
-      <c r="J20" s="23">
-        <f t="shared" ref="J20" si="1">F20/G20</f>
+      <c r="J28" s="23">
+        <f t="shared" ref="J28" si="1">F28/G28</f>
         <v>0.7767015233582597</v>
       </c>
-      <c r="K20" s="24">
-        <f>G20/H20</f>
+      <c r="K28" s="24">
+        <f>G28/H28</f>
         <v>1.1426665023005744</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
-      <c r="B21" s="75" t="s">
+    <row r="29" spans="1:11">
+      <c r="B29" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="76"/>
-      <c r="G21" s="76"/>
-      <c r="H21" s="76"/>
-      <c r="I21" s="76"/>
-      <c r="J21" s="76"/>
-      <c r="K21" s="77"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="B22" s="63"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
-      <c r="K22" s="65"/>
-    </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1">
-      <c r="B23" s="60"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="62"/>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="76"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="76"/>
+      <c r="I29" s="76"/>
+      <c r="J29" s="76"/>
+      <c r="K29" s="77"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="B30" s="63"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="64"/>
+      <c r="H30" s="64"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="64"/>
+      <c r="K30" s="65"/>
+    </row>
+    <row r="31" spans="1:11" ht="15" thickBot="1">
+      <c r="B31" s="60"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="61"/>
+      <c r="K31" s="62"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B23:K23"/>
-    <mergeCell ref="B22:K22"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="B30:K30"/>
     <mergeCell ref="B1:K1"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B21:K21"/>
+    <mergeCell ref="B29:K29"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:K2"/>

</xml_diff>